<commit_message>
Ar - securitas direct
</commit_message>
<xml_diff>
--- a/Herramientas y Documentacion/Documentación Permisos.xlsx
+++ b/Herramientas y Documentacion/Documentación Permisos.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28125" windowHeight="12495"/>
+    <workbookView windowWidth="31245" windowHeight="17055"/>
   </bookViews>
   <sheets>
     <sheet name="Metodos permisos inserts" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="698" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="704" uniqueCount="235">
   <si>
     <t>Servicio / Interfaz</t>
   </si>
@@ -594,10 +594,19 @@
     <t>employeePhoto</t>
   </si>
   <si>
-    <t>com.ontimize.atomicHotelsApiRest.api.core.service.IEmployeePhoto/</t>
+    <t>com.ontimize.atomicHotelsApiRest.api.core.service.IEmployeePhotoService/</t>
+  </si>
+  <si>
+    <t>/employeephoto/employeePhoto</t>
+  </si>
+  <si>
+    <t>employeePhotoDelete</t>
   </si>
   <si>
     <t>getPicture</t>
+  </si>
+  <si>
+    <t>/employeephoto/getPicture</t>
   </si>
   <si>
     <t>ROLES</t>
@@ -725,10 +734,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_-* #,##0\ &quot;€&quot;_-;\-* #,##0\ &quot;€&quot;_-;_-* &quot;-&quot;\ &quot;€&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="176" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* \-??\ &quot;€&quot;_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-* #,##0\ &quot;€&quot;_-;\-* #,##0\ &quot;€&quot;_-;_-* &quot;-&quot;\ &quot;€&quot;_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* \-??\ &quot;€&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -778,6 +787,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -792,8 +808,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -815,19 +839,18 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -862,20 +885,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
@@ -893,15 +902,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -914,8 +922,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -930,7 +939,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -942,7 +975,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -960,7 +999,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -972,7 +1059,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -984,109 +1095,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1104,13 +1119,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1148,6 +1157,30 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1174,30 +1207,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1239,19 +1248,19 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1260,127 +1269,127 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1744,8 +1753,8 @@
   <sheetPr/>
   <dimension ref="A1:J277"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H38" sqref="H38"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="F56" sqref="F56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15"/>
@@ -5544,20 +5553,23 @@
         <v>121</v>
       </c>
       <c r="D176" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="E176" s="1" t="s">
-        <v>16</v>
+        <v>100</v>
+      </c>
+      <c r="G176" s="1" t="s">
+        <v>191</v>
       </c>
       <c r="J176" s="13" t="str">
         <f>IF(B176&lt;&gt;"",CONCATENATE(inicio_consulta,C176,mid_consulta,A176,B176,fin_consulta),IF(A176&lt;&gt;"",CONCATENATE("-- ",A176),""))</f>
-        <v>INSERT INTO tserver_permission VALUES (121,'com.ontimize.atomicHotelsApiRest.api.core.service.IEmployeePhoto/employeePhotoQuery');</v>
+        <v>INSERT INTO tserver_permission VALUES (121,'com.ontimize.atomicHotelsApiRest.api.core.service.IEmployeePhotoService/employeePhotoQuery');</v>
       </c>
     </row>
     <row r="177" spans="1:10">
       <c r="A177" s="1" t="str">
         <f>A176</f>
-        <v>com.ontimize.atomicHotelsApiRest.api.core.service.IEmployeePhoto/</v>
+        <v>com.ontimize.atomicHotelsApiRest.api.core.service.IEmployeePhotoService/</v>
       </c>
       <c r="B177" s="1" t="str">
         <f>IF(A175&lt;&gt;"",CONCATENATE(A175,"Insert"),"")</f>
@@ -5568,85 +5580,78 @@
         <v>122</v>
       </c>
       <c r="D177" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="E177" s="1" t="s">
-        <v>16</v>
+        <v>100</v>
+      </c>
+      <c r="G177" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="H177" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="J177" s="13" t="str">
         <f>IF(B177&lt;&gt;"",CONCATENATE(inicio_consulta,C177,mid_consulta,A177,B177,fin_consulta),IF(A177&lt;&gt;"",CONCATENATE("-- ",A177),""))</f>
-        <v>INSERT INTO tserver_permission VALUES (122,'com.ontimize.atomicHotelsApiRest.api.core.service.IEmployeePhoto/employeePhotoInsert');</v>
+        <v>INSERT INTO tserver_permission VALUES (122,'com.ontimize.atomicHotelsApiRest.api.core.service.IEmployeePhotoService/employeePhotoInsert');</v>
       </c>
     </row>
     <row r="178" spans="1:10">
       <c r="A178" s="1" t="str">
         <f>A177</f>
-        <v>com.ontimize.atomicHotelsApiRest.api.core.service.IEmployeePhoto/</v>
-      </c>
-      <c r="B178" s="1" t="str">
-        <f>IF(A175&lt;&gt;"",CONCATENATE(A175,"Update"),"")</f>
-        <v>employeePhotoUpdate</v>
+        <v>com.ontimize.atomicHotelsApiRest.api.core.service.IEmployeePhotoService/</v>
+      </c>
+      <c r="B178" s="1" t="s">
+        <v>192</v>
       </c>
       <c r="C178" s="12">
         <f t="shared" si="24"/>
         <v>123</v>
       </c>
       <c r="D178" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="E178" s="1" t="s">
-        <v>16</v>
+        <v>100</v>
+      </c>
+      <c r="G178" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="H178" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="J178" s="13" t="str">
         <f>IF(B178&lt;&gt;"",CONCATENATE(inicio_consulta,C178,mid_consulta,A178,B178,fin_consulta),IF(A178&lt;&gt;"",CONCATENATE("-- ",A178),""))</f>
-        <v>INSERT INTO tserver_permission VALUES (123,'com.ontimize.atomicHotelsApiRest.api.core.service.IEmployeePhoto/employeePhotoUpdate');</v>
+        <v>INSERT INTO tserver_permission VALUES (123,'com.ontimize.atomicHotelsApiRest.api.core.service.IEmployeePhotoService/employeePhotoDelete');</v>
       </c>
     </row>
     <row r="179" spans="1:10">
       <c r="A179" s="1" t="str">
         <f>A178</f>
-        <v>com.ontimize.atomicHotelsApiRest.api.core.service.IEmployeePhoto/</v>
-      </c>
-      <c r="B179" s="1" t="str">
-        <f>IF(A175&lt;&gt;"",CONCATENATE(A175,"Delete"),"")</f>
-        <v>employeePhotoDelete</v>
+        <v>com.ontimize.atomicHotelsApiRest.api.core.service.IEmployeePhotoService/</v>
+      </c>
+      <c r="B179" s="1" t="s">
+        <v>193</v>
       </c>
       <c r="C179" s="12">
         <f t="shared" si="24"/>
         <v>124</v>
       </c>
       <c r="D179" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="E179" s="1" t="s">
-        <v>16</v>
+        <v>100</v>
+      </c>
+      <c r="G179" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="H179" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="J179" s="13" t="str">
         <f>IF(B179&lt;&gt;"",CONCATENATE(inicio_consulta,C179,mid_consulta,A179,B179,fin_consulta),IF(A179&lt;&gt;"",CONCATENATE("-- ",A179),""))</f>
-        <v>INSERT INTO tserver_permission VALUES (124,'com.ontimize.atomicHotelsApiRest.api.core.service.IEmployeePhoto/employeePhotoDelete');</v>
-      </c>
-    </row>
-    <row r="180" spans="1:10">
-      <c r="A180" s="1" t="str">
-        <f>A179</f>
-        <v>com.ontimize.atomicHotelsApiRest.api.core.service.IEmployeePhoto/</v>
-      </c>
-      <c r="B180" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="C180" s="12">
-        <f t="shared" si="24"/>
-        <v>125</v>
-      </c>
-      <c r="D180" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E180" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J180" s="13" t="str">
-        <f>IF(B180&lt;&gt;"",CONCATENATE(inicio_consulta,C180,mid_consulta,A180,B180,fin_consulta),IF(A180&lt;&gt;"",CONCATENATE("-- ",A180),""))</f>
-        <v>INSERT INTO tserver_permission VALUES (125,'com.ontimize.atomicHotelsApiRest.api.core.service.IEmployeePhoto/getPicture');</v>
+        <v>INSERT INTO tserver_permission VALUES (124,'com.ontimize.atomicHotelsApiRest.api.core.service.IEmployeePhotoService/getPicture');</v>
       </c>
     </row>
     <row r="181" spans="10:10">
@@ -6261,12 +6266,12 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="2" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
       <c r="F1" s="2" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
@@ -6274,29 +6279,29 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="2" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="2" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -6304,16 +6309,16 @@
         <v>0</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="G3" s="6">
         <v>123456</v>
@@ -6328,16 +6333,16 @@
         <v>1</v>
       </c>
       <c r="B4" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>203</v>
-      </c>
       <c r="D4" s="4" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="G4" s="6">
         <v>123456</v>
@@ -6352,25 +6357,25 @@
         <v>2</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="G5" s="6">
         <v>123456</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -6378,25 +6383,25 @@
         <v>3</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="G6" s="6">
         <v>123456</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -6407,22 +6412,22 @@
         <v>76</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="G7" s="6">
         <v>123456</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -6433,59 +6438,59 @@
         <v>139</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="G8" s="6">
         <v>123456</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="I8" s="9" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
     </row>
     <row r="9" spans="6:9">
       <c r="F9" s="6" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="G9" s="6">
         <v>123456</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="I9" s="9"/>
     </row>
     <row r="10" spans="6:9">
       <c r="F10" s="4" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="G10" s="6">
         <v>123456</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
     </row>
     <row r="11" spans="6:9">
       <c r="F11" s="6" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="G11" s="6">
         <v>123456</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="I11" s="9"/>
     </row>
@@ -6521,7 +6526,7 @@
   <sheetData>
     <row r="1" spans="2:2">
       <c r="B1" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
     </row>
     <row r="2" spans="2:3">
@@ -6534,7 +6539,7 @@
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
     </row>
     <row r="7" spans="2:5">
@@ -7495,17 +7500,17 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="19" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="19" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
     </row>
   </sheetData>

</xml_diff>